<commit_message>
clinton leggin DDL, docker compose files added
</commit_message>
<xml_diff>
--- a/spring-class-7/tables identified.xlsx
+++ b/spring-class-7/tables identified.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YOGA\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YOGA\Documents\codes\pondit-b5\spring-class-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E569B87-9581-49AF-B563-AC1CF159AE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBE313D-9991-46A4-ACB1-F61421556DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{565D94D5-5459-4181-94D2-1647BF522C4C}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{565D94D5-5459-4181-94D2-1647BF522C4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>Property</t>
   </si>
@@ -145,6 +146,144 @@
   </si>
   <si>
     <t>Part_quantity</t>
+  </si>
+  <si>
+    <t>Client Table</t>
+  </si>
+  <si>
+    <t>Portfolio Table</t>
+  </si>
+  <si>
+    <t>Property Table</t>
+  </si>
+  <si>
+    <t>Address Table</t>
+  </si>
+  <si>
+    <t>Property Type Table</t>
+  </si>
+  <si>
+    <t>Tenant Table</t>
+  </si>
+  <si>
+    <t>Tenancy Table</t>
+  </si>
+  <si>
+    <t>Client ID (P)</t>
+  </si>
+  <si>
+    <t>Portfolio ID (P)</t>
+  </si>
+  <si>
+    <t>Property ID (P)</t>
+  </si>
+  <si>
+    <t>Address ID (P)</t>
+  </si>
+  <si>
+    <t>Property Type ID (P)</t>
+  </si>
+  <si>
+    <t>Tenant ID (P)</t>
+  </si>
+  <si>
+    <t>Tenancy ID (P)</t>
+  </si>
+  <si>
+    <t>Client Name</t>
+  </si>
+  <si>
+    <t>Client ID (F)</t>
+  </si>
+  <si>
+    <t>Address ID (F)</t>
+  </si>
+  <si>
+    <t>Address Number</t>
+  </si>
+  <si>
+    <t>Property Type</t>
+  </si>
+  <si>
+    <t>Tenant Name</t>
+  </si>
+  <si>
+    <t>Tenant ID (F)</t>
+  </si>
+  <si>
+    <t>Property ID (F)</t>
+  </si>
+  <si>
+    <t>Property Type ID (F)</t>
+  </si>
+  <si>
+    <t>Street ID</t>
+  </si>
+  <si>
+    <t>Tenant Type</t>
+  </si>
+  <si>
+    <t>Postal ID</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Monthly Rent</t>
+  </si>
+  <si>
+    <t>Part Table</t>
+  </si>
+  <si>
+    <t>Staff Table</t>
+  </si>
+  <si>
+    <t>Repair Table</t>
+  </si>
+  <si>
+    <t>Part Used Table</t>
+  </si>
+  <si>
+    <t>Part ID (P)</t>
+  </si>
+  <si>
+    <t>Staff ID (P)</t>
+  </si>
+  <si>
+    <t>Repair ID (P)</t>
+  </si>
+  <si>
+    <t>Part Used ID (P)</t>
+  </si>
+  <si>
+    <t>Part Code</t>
+  </si>
+  <si>
+    <t>Staff Name</t>
+  </si>
+  <si>
+    <t>Repair ID (F)</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>Part ID (F)</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Repair Staff Table</t>
+  </si>
+  <si>
+    <t>Repair Staff ID (P)</t>
+  </si>
+  <si>
+    <t>Staff ID (F)</t>
   </si>
 </sst>
 </file>
@@ -233,10 +372,8 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -251,6 +388,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -567,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3351F433-D73D-42EB-8996-10336EBD5BDC}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -583,24 +726,18 @@
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -611,7 +748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -622,7 +759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -630,18 +767,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="1:7">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:7">
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -652,7 +789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:7">
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -663,8 +800,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
@@ -674,7 +811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -682,27 +819,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="E13" s="3" t="s">
+    <row r="13" spans="1:7">
+      <c r="E13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:7">
       <c r="E14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:7">
       <c r="E15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:7">
       <c r="E16" t="s">
         <v>21</v>
       </c>
@@ -723,76 +860,504 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1"/>
-    <row r="22" spans="1:5" ht="27.6" thickBot="1">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:5" ht="15" thickBot="1">
+      <c r="A22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="27.6" thickBot="1">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:5" ht="15" thickBot="1">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="27.6" thickBot="1">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:5" ht="15" thickBot="1">
+      <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="6" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="27.6" thickBot="1">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6" t="s">
+    <row r="26" spans="1:5" ht="15" thickBot="1">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="6" t="s">
+      <c r="A27" s="4"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="4" t="s">
         <v>33</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330451BD-F824-4656-A59B-4B757ED0CF0E}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="40.799999999999997" thickBot="1">
+      <c r="A1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" ht="40.799999999999997" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="27.6" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="40.799999999999997" thickBot="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" ht="27.6" thickBot="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" ht="27.6" thickBot="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" ht="40.799999999999997" thickBot="1">
+      <c r="A8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" ht="40.799999999999997" thickBot="1">
+      <c r="A9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" ht="27.6" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" ht="27.6" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1">
+      <c r="A15" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1">
+      <c r="A16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" ht="27.6" thickBot="1">
+      <c r="A17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="27.6" thickBot="1">
+      <c r="A18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickBot="1">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" thickBot="1">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>